<commit_message>
vehicle-km and occupancy rate now time-dependent.
</commit_message>
<xml_diff>
--- a/RECC_Config_V2_4.xlsx
+++ b/RECC_Config_V2_4.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12491" uniqueCount="808">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12491" uniqueCount="810">
   <si>
     <t>User Name</t>
   </si>
@@ -1822,12 +1822,6 @@
     <t>V4.1</t>
   </si>
   <si>
-    <t>b8369ae7-71b4-4acb-9d38-ca997d3d211f</t>
-  </si>
-  <si>
-    <t>95309e7e-ef30-40ca-af35-75e647b4ddb9</t>
-  </si>
-  <si>
     <t>54a8e373-bcef-4967-9590-6049061c48c7</t>
   </si>
   <si>
@@ -2456,6 +2450,18 @@
   </si>
   <si>
     <t>passenger vehicles. future development of per capita product stock. none. none. none. (this info extracted from the target table excel sheet, refer to it for details.)</t>
+  </si>
+  <si>
+    <t>V4.2</t>
+  </si>
+  <si>
+    <t>e97f26de-e3cc-444f-b98a-9d1455be54b1</t>
+  </si>
+  <si>
+    <t>227ee5a9-5cf3-47bd-9f3c-df5adb1ba966</t>
+  </si>
+  <si>
+    <t>3e3e00b2-1b18-459f-87e1-014aeb1850d4</t>
   </si>
 </sst>
 </file>
@@ -3337,7 +3343,7 @@
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="45" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="G4" s="23"/>
     </row>
@@ -4101,7 +4107,7 @@
         <v>256</v>
       </c>
       <c r="D4" s="95" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.45">
@@ -4109,7 +4115,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="95" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.45">
@@ -4125,7 +4131,7 @@
         <v>261</v>
       </c>
       <c r="D7" s="93" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="E7" t="s">
         <v>263</v>
@@ -4335,7 +4341,7 @@
         <v>287</v>
       </c>
       <c r="G21" s="93" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="H21" s="34" t="s">
         <v>47</v>
@@ -7679,7 +7685,7 @@
         <v>256</v>
       </c>
       <c r="D4" s="95" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.45">
@@ -7687,7 +7693,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="95" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.45">
@@ -7703,7 +7709,7 @@
         <v>261</v>
       </c>
       <c r="D7" s="93" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="E7" t="s">
         <v>263</v>
@@ -7913,7 +7919,7 @@
         <v>287</v>
       </c>
       <c r="G21" s="93" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="H21" s="34" t="s">
         <v>47</v>
@@ -11257,7 +11263,7 @@
         <v>256</v>
       </c>
       <c r="D4" s="95" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.45">
@@ -11265,7 +11271,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="95" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.45">
@@ -11281,7 +11287,7 @@
         <v>261</v>
       </c>
       <c r="D7" s="93" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="E7" t="s">
         <v>263</v>
@@ -11491,7 +11497,7 @@
         <v>287</v>
       </c>
       <c r="G21" s="93" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="H21" s="34" t="s">
         <v>47</v>
@@ -14835,7 +14841,7 @@
         <v>256</v>
       </c>
       <c r="D4" s="95" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.45">
@@ -14843,7 +14849,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="95" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.45">
@@ -14859,7 +14865,7 @@
         <v>261</v>
       </c>
       <c r="D7" s="93" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="E7" t="s">
         <v>263</v>
@@ -15069,7 +15075,7 @@
         <v>287</v>
       </c>
       <c r="G21" s="93" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="H21" s="34" t="s">
         <v>47</v>
@@ -18413,7 +18419,7 @@
         <v>256</v>
       </c>
       <c r="D4" s="95" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.45">
@@ -18421,7 +18427,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="95" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.45">
@@ -18437,7 +18443,7 @@
         <v>261</v>
       </c>
       <c r="D7" s="93" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="E7" t="s">
         <v>263</v>
@@ -18647,7 +18653,7 @@
         <v>287</v>
       </c>
       <c r="G21" s="93" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="H21" s="34" t="s">
         <v>47</v>
@@ -23535,8 +23541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -23587,7 +23593,7 @@
         <v>256</v>
       </c>
       <c r="D4" s="95" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.45">
@@ -23595,7 +23601,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="95" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.45">
@@ -23603,7 +23609,7 @@
         <v>259</v>
       </c>
       <c r="D6" s="95" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.45">
@@ -23611,7 +23617,7 @@
         <v>261</v>
       </c>
       <c r="D7" s="93" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E7" s="48" t="s">
         <v>263</v>
@@ -23821,7 +23827,7 @@
         <v>287</v>
       </c>
       <c r="G21" s="93" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="H21" s="34" t="s">
         <v>47</v>
@@ -23960,7 +23966,7 @@
         <v>302</v>
       </c>
       <c r="G27" s="93" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="H27" s="34" t="s">
         <v>81</v>
@@ -23983,7 +23989,7 @@
         <v>85</v>
       </c>
       <c r="G28" s="93" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="H28" s="34" t="s">
         <v>88</v>
@@ -24006,7 +24012,7 @@
         <v>307</v>
       </c>
       <c r="G29" s="93" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="H29" s="34" t="s">
         <v>95</v>
@@ -24089,7 +24095,7 @@
         <v>117</v>
       </c>
       <c r="D33" s="93" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E33" s="93" t="s">
         <v>87</v>
@@ -24098,7 +24104,7 @@
         <v>316</v>
       </c>
       <c r="G33" s="93" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="H33" s="34" t="s">
         <v>119</v>
@@ -24213,7 +24219,7 @@
         <v>326</v>
       </c>
       <c r="G38" s="93" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="H38" s="34" t="s">
         <v>146</v>
@@ -24282,7 +24288,7 @@
         <v>334</v>
       </c>
       <c r="G41" s="93" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="H41" s="34" t="s">
         <v>164</v>
@@ -24431,94 +24437,94 @@
     </row>
     <row r="48" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C48" s="33" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D48" s="93" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="E48" s="93" t="s">
         <v>87</v>
       </c>
       <c r="F48" s="93" t="s">
+        <v>685</v>
+      </c>
+      <c r="G48" s="93" t="s">
+        <v>736</v>
+      </c>
+      <c r="H48" s="34" t="s">
+        <v>686</v>
+      </c>
+      <c r="I48" s="93" t="s">
         <v>687</v>
-      </c>
-      <c r="G48" s="93" t="s">
-        <v>738</v>
-      </c>
-      <c r="H48" s="34" t="s">
-        <v>688</v>
-      </c>
-      <c r="I48" s="93" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C49" s="33" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="D49" s="93" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E49" s="93" t="s">
         <v>87</v>
       </c>
       <c r="F49" s="93" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G49" s="93" t="s">
         <v>285</v>
       </c>
       <c r="H49" s="34" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="I49" s="93" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C50" s="33" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D50" s="93" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="E50" s="93" t="s">
         <v>87</v>
       </c>
       <c r="F50" s="93" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G50" s="93" t="s">
         <v>285</v>
       </c>
       <c r="H50" s="34" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="I50" s="93" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C51" s="33" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="D51" s="93" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="E51" s="93" t="s">
         <v>162</v>
       </c>
       <c r="F51" s="93" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="G51" s="93" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="H51" s="34" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="I51" s="93" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.45">
@@ -24861,7 +24867,7 @@
         <v>340</v>
       </c>
       <c r="I77" s="48" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="J77" s="48" t="s">
         <v>391</v>
@@ -24896,7 +24902,7 @@
         <v>340</v>
       </c>
       <c r="I78" s="48" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="J78" s="48" t="s">
         <v>391</v>
@@ -24984,16 +24990,16 @@
         <v>364</v>
       </c>
       <c r="C81" s="94" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="D81" s="93" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="E81" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F81" s="37" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="G81" s="93" t="s">
         <v>410</v>
@@ -25002,7 +25008,7 @@
         <v>340</v>
       </c>
       <c r="I81" s="30" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="J81" s="48" t="s">
         <v>395</v>
@@ -25018,16 +25024,16 @@
         <v>364</v>
       </c>
       <c r="C82" s="94" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="D82" s="93" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="E82" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F82" s="37" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="G82" s="93" t="s">
         <v>410</v>
@@ -25036,7 +25042,7 @@
         <v>340</v>
       </c>
       <c r="I82" s="30" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="J82" s="48" t="s">
         <v>395</v>
@@ -25052,16 +25058,16 @@
         <v>364</v>
       </c>
       <c r="C83" s="94" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D83" s="93" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E83" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F83" s="37" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="G83" s="93" t="s">
         <v>338</v>
@@ -25070,7 +25076,7 @@
         <v>340</v>
       </c>
       <c r="I83" s="30" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="J83" s="48" t="s">
         <v>395</v>
@@ -25086,13 +25092,13 @@
         <v>364</v>
       </c>
       <c r="C84" s="94" t="s">
+        <v>803</v>
+      </c>
+      <c r="D84" s="93" t="s">
         <v>805</v>
       </c>
-      <c r="D84" s="93" t="s">
-        <v>807</v>
-      </c>
       <c r="E84" s="93" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="F84" s="37" t="s">
         <v>41</v>
@@ -25104,7 +25110,7 @@
         <v>340</v>
       </c>
       <c r="I84" s="30" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="J84" s="48" t="s">
         <v>395</v>
@@ -25140,7 +25146,7 @@
         <v>340</v>
       </c>
       <c r="I85" s="30" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="J85" s="48" t="s">
         <v>388</v>
@@ -25280,7 +25286,7 @@
         <v>340</v>
       </c>
       <c r="I89" s="50" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="J89" s="50" t="s">
         <v>388</v>
@@ -25319,7 +25325,7 @@
         <v>340</v>
       </c>
       <c r="I90" s="48" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="J90" s="50" t="s">
         <v>388</v>
@@ -25432,7 +25438,7 @@
         <v>340</v>
       </c>
       <c r="I93" s="48" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="J93" s="48" t="s">
         <v>391</v>
@@ -25573,7 +25579,7 @@
         <v>340</v>
       </c>
       <c r="I97" s="48" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="J97" s="48" t="s">
         <v>391</v>
@@ -25625,10 +25631,10 @@
         <v>364</v>
       </c>
       <c r="C99" s="94" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D99" s="93" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E99" s="93" t="s">
         <v>55</v>
@@ -25643,7 +25649,7 @@
         <v>340</v>
       </c>
       <c r="I99" s="48" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="J99" s="48" t="s">
         <v>391</v>
@@ -25660,10 +25666,10 @@
         <v>364</v>
       </c>
       <c r="C100" s="94" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="D100" s="93" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="E100" s="93" t="s">
         <v>55</v>
@@ -25678,7 +25684,7 @@
         <v>340</v>
       </c>
       <c r="I100" s="48" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="J100" s="48" t="s">
         <v>391</v>
@@ -25695,16 +25701,16 @@
         <v>364</v>
       </c>
       <c r="C101" s="94" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="D101" s="93" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="E101" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F101" s="37" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="G101" s="93" t="s">
         <v>333</v>
@@ -25713,7 +25719,7 @@
         <v>340</v>
       </c>
       <c r="I101" s="48" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="J101" s="48" t="s">
         <v>391</v>
@@ -25757,7 +25763,6 @@
         <v>110</v>
       </c>
       <c r="L102" s="50"/>
-      <c r="M102" s="50"/>
       <c r="N102" s="50"/>
       <c r="O102" s="50"/>
     </row>
@@ -25787,7 +25792,7 @@
         <v>340</v>
       </c>
       <c r="I103" s="50" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="J103" s="50" t="s">
         <v>391</v>
@@ -25796,7 +25801,6 @@
         <v>104</v>
       </c>
       <c r="L103" s="50"/>
-      <c r="M103" s="50"/>
       <c r="N103" s="50"/>
       <c r="O103" s="50"/>
     </row>
@@ -25835,7 +25839,6 @@
         <v>104</v>
       </c>
       <c r="L104" s="50"/>
-      <c r="M104" s="50"/>
       <c r="N104" s="50"/>
       <c r="O104" s="50"/>
     </row>
@@ -25847,16 +25850,16 @@
         <v>364</v>
       </c>
       <c r="C105" s="94" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="D105" s="98" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="E105" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F105" s="41" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="G105" s="93" t="s">
         <v>338</v>
@@ -25865,7 +25868,7 @@
         <v>340</v>
       </c>
       <c r="I105" s="48" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="J105" s="50" t="s">
         <v>391</v>
@@ -25874,7 +25877,6 @@
         <v>104</v>
       </c>
       <c r="L105" s="50"/>
-      <c r="M105" s="50"/>
       <c r="N105" s="50"/>
       <c r="O105" s="50"/>
     </row>
@@ -25886,16 +25888,16 @@
         <v>364</v>
       </c>
       <c r="C106" s="94" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="D106" s="98" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E106" s="93" t="s">
         <v>28</v>
       </c>
       <c r="F106" s="41" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="G106" s="93" t="s">
         <v>338</v>
@@ -25904,14 +25906,13 @@
         <v>340</v>
       </c>
       <c r="I106" s="48" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="J106" s="50" t="s">
         <v>391</v>
       </c>
       <c r="K106" s="50"/>
       <c r="L106" s="50"/>
-      <c r="M106" s="50"/>
       <c r="N106" s="50"/>
       <c r="O106" s="50"/>
     </row>
@@ -25923,16 +25924,16 @@
         <v>364</v>
       </c>
       <c r="C107" s="94" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="D107" s="98" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="E107" s="93" t="s">
         <v>28</v>
       </c>
       <c r="F107" s="41" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="G107" s="93" t="s">
         <v>333</v>
@@ -25941,7 +25942,7 @@
         <v>340</v>
       </c>
       <c r="I107" s="26" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="J107" s="50" t="s">
         <v>391</v>
@@ -25978,7 +25979,7 @@
         <v>340</v>
       </c>
       <c r="I108" s="48" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="J108" s="48" t="s">
         <v>391</v>
@@ -26013,7 +26014,7 @@
         <v>340</v>
       </c>
       <c r="I109" s="48" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="J109" s="48" t="s">
         <v>391</v>
@@ -26109,7 +26110,7 @@
         <v>431</v>
       </c>
       <c r="E112" s="93" t="s">
-        <v>595</v>
+        <v>806</v>
       </c>
       <c r="F112" s="39" t="s">
         <v>137</v>
@@ -26120,8 +26121,8 @@
       <c r="H112" s="93" t="s">
         <v>340</v>
       </c>
-      <c r="I112" s="96" t="s">
-        <v>596</v>
+      <c r="I112" s="50" t="s">
+        <v>807</v>
       </c>
       <c r="J112" s="48" t="s">
         <v>395</v>
@@ -26144,7 +26145,7 @@
         <v>433</v>
       </c>
       <c r="E113" s="93" t="s">
-        <v>97</v>
+        <v>595</v>
       </c>
       <c r="F113" s="37" t="s">
         <v>143</v>
@@ -26155,8 +26156,8 @@
       <c r="H113" s="93" t="s">
         <v>340</v>
       </c>
-      <c r="I113" s="48" t="s">
-        <v>434</v>
+      <c r="I113" s="50" t="s">
+        <v>808</v>
       </c>
       <c r="J113" s="48" t="s">
         <v>395</v>
@@ -26179,7 +26180,7 @@
         <v>435</v>
       </c>
       <c r="E114" s="93" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="F114" s="37" t="s">
         <v>148</v>
@@ -26190,8 +26191,8 @@
       <c r="H114" s="93" t="s">
         <v>340</v>
       </c>
-      <c r="I114" s="48" t="s">
-        <v>597</v>
+      <c r="I114" s="50" t="s">
+        <v>809</v>
       </c>
       <c r="J114" s="48" t="s">
         <v>395</v>
@@ -26296,7 +26297,7 @@
         <v>340</v>
       </c>
       <c r="I117" s="48" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="J117" s="48" t="s">
         <v>391</v>
@@ -26319,7 +26320,7 @@
         <v>445</v>
       </c>
       <c r="E118" s="93" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="F118" s="37" t="s">
         <v>172</v>
@@ -26331,7 +26332,7 @@
         <v>340</v>
       </c>
       <c r="I118" s="48" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="J118" s="48" t="s">
         <v>391</v>
@@ -26366,7 +26367,7 @@
         <v>340</v>
       </c>
       <c r="I119" s="48" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="J119" s="48" t="s">
         <v>391</v>
@@ -26508,7 +26509,7 @@
         <v>340</v>
       </c>
       <c r="I123" s="48" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="J123" s="55" t="s">
         <v>457</v>
@@ -26597,16 +26598,16 @@
         <v>364</v>
       </c>
       <c r="C126" s="94" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D126" s="93" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E126" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F126" s="37" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="G126" s="93" t="s">
         <v>338</v>
@@ -26615,7 +26616,7 @@
         <v>340</v>
       </c>
       <c r="I126" s="48" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="J126" s="55" t="s">
         <v>457</v>
@@ -26708,10 +26709,10 @@
         <v>206</v>
       </c>
       <c r="D129" s="93" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E129" s="93" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="F129" s="37" t="s">
         <v>207</v>
@@ -26723,7 +26724,7 @@
         <v>340</v>
       </c>
       <c r="I129" s="48" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="J129" s="55" t="s">
         <v>457</v>
@@ -26744,7 +26745,7 @@
         <v>208</v>
       </c>
       <c r="D130" s="93" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="E130" s="93" t="s">
         <v>40</v>
@@ -26777,16 +26778,16 @@
         <v>444</v>
       </c>
       <c r="C131" s="94" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D131" s="93" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="E131" s="93" t="s">
         <v>28</v>
       </c>
       <c r="F131" s="37" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="G131" s="93" t="s">
         <v>333</v>
@@ -26795,7 +26796,7 @@
         <v>340</v>
       </c>
       <c r="I131" s="48" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="J131" s="55" t="s">
         <v>457</v>
@@ -26831,7 +26832,7 @@
         <v>340</v>
       </c>
       <c r="I132" s="48" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="J132" s="48" t="s">
         <v>391</v>
@@ -26938,7 +26939,7 @@
         <v>340</v>
       </c>
       <c r="I135" s="48" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="J135" s="48" t="s">
         <v>395</v>
@@ -26973,7 +26974,7 @@
         <v>340</v>
       </c>
       <c r="I136" s="30" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="J136" s="48" t="s">
         <v>395</v>
@@ -26990,7 +26991,7 @@
         <v>364</v>
       </c>
       <c r="C137" s="94" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D137" s="95" t="s">
         <v>475</v>
@@ -26999,7 +27000,7 @@
         <v>55</v>
       </c>
       <c r="F137" s="37" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="G137" s="93" t="s">
         <v>386</v>
@@ -27008,7 +27009,7 @@
         <v>340</v>
       </c>
       <c r="I137" s="30" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="J137" s="48" t="s">
         <v>395</v>
@@ -27063,7 +27064,7 @@
         <v>222</v>
       </c>
       <c r="D139" s="95" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E139" s="93" t="s">
         <v>238</v>
@@ -27078,7 +27079,7 @@
         <v>340</v>
       </c>
       <c r="I139" s="48" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J139" s="48" t="s">
         <v>395</v>
@@ -27095,10 +27096,10 @@
         <v>364</v>
       </c>
       <c r="C140" s="94" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D140" s="95" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E140" s="93" t="s">
         <v>55</v>
@@ -27113,7 +27114,7 @@
         <v>340</v>
       </c>
       <c r="I140" s="48" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J140" s="48" t="s">
         <v>395</v>
@@ -27183,7 +27184,7 @@
         <v>340</v>
       </c>
       <c r="I142" s="48" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="J142" s="48" t="s">
         <v>395</v>
@@ -27200,10 +27201,10 @@
         <v>364</v>
       </c>
       <c r="C143" s="94" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D143" s="93" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="E143" s="93" t="s">
         <v>55</v>
@@ -27218,7 +27219,7 @@
         <v>340</v>
       </c>
       <c r="I143" s="48" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="J143" s="48" t="s">
         <v>395</v>
@@ -27288,7 +27289,7 @@
         <v>340</v>
       </c>
       <c r="I145" s="48" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="J145" s="48" t="s">
         <v>395</v>
@@ -27305,10 +27306,10 @@
         <v>364</v>
       </c>
       <c r="C146" s="94" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D146" s="93" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="E146" s="93" t="s">
         <v>55</v>
@@ -27323,7 +27324,7 @@
         <v>340</v>
       </c>
       <c r="I146" s="48" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="J146" s="48" t="s">
         <v>395</v>
@@ -27393,7 +27394,7 @@
         <v>340</v>
       </c>
       <c r="I148" s="30" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="J148" s="48" t="s">
         <v>395</v>
@@ -27481,10 +27482,10 @@
         <v>364</v>
       </c>
       <c r="C151" s="94" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D151" s="42" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="E151" s="93" t="s">
         <v>55</v>
@@ -27499,7 +27500,7 @@
         <v>340</v>
       </c>
       <c r="I151" s="97" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="J151" s="48" t="s">
         <v>395</v>
@@ -27516,10 +27517,10 @@
         <v>364</v>
       </c>
       <c r="C152" s="94" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D152" s="42" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E152" s="93" t="s">
         <v>55</v>
@@ -27534,7 +27535,7 @@
         <v>340</v>
       </c>
       <c r="I152" s="30" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="J152" s="48" t="s">
         <v>395</v>
@@ -27557,7 +27558,7 @@
         <v>498</v>
       </c>
       <c r="E153" s="93" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="F153" s="37" t="s">
         <v>247</v>
@@ -27569,7 +27570,7 @@
         <v>340</v>
       </c>
       <c r="I153" s="48" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="J153" s="48" t="s">
         <v>391</v>
@@ -27691,16 +27692,16 @@
         <v>444</v>
       </c>
       <c r="C157" s="94" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="D157" s="43" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="E157" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F157" s="37" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="G157" s="93" t="s">
         <v>333</v>
@@ -27709,13 +27710,13 @@
         <v>340</v>
       </c>
       <c r="I157" s="48" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="J157" s="48" t="s">
         <v>391</v>
       </c>
       <c r="K157" s="55" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.45">
@@ -27723,13 +27724,13 @@
         <v>82</v>
       </c>
       <c r="B158" s="53" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C158" s="94" t="s">
+        <v>776</v>
+      </c>
+      <c r="D158" s="43" t="s">
         <v>778</v>
-      </c>
-      <c r="D158" s="43" t="s">
-        <v>780</v>
       </c>
       <c r="E158" s="93" t="s">
         <v>55</v>
@@ -27744,10 +27745,10 @@
         <v>340</v>
       </c>
       <c r="I158" s="48" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="J158" s="48" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="K158" s="55" t="s">
         <v>92</v>
@@ -27758,13 +27759,13 @@
         <v>83</v>
       </c>
       <c r="B159" s="53" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C159" s="94" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="D159" s="43" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="E159" s="93" t="s">
         <v>55</v>
@@ -27779,10 +27780,10 @@
         <v>340</v>
       </c>
       <c r="I159" s="48" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="J159" s="48" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="K159" s="55" t="s">
         <v>92</v>
@@ -27796,16 +27797,16 @@
         <v>444</v>
       </c>
       <c r="C160" s="94" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D160" s="43" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="E160" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F160" s="37" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="G160" s="93" t="s">
         <v>338</v>
@@ -27814,7 +27815,7 @@
         <v>340</v>
       </c>
       <c r="I160" s="26" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="J160" s="48" t="s">
         <v>391</v>
@@ -27831,16 +27832,16 @@
         <v>430</v>
       </c>
       <c r="C161" s="94" t="s">
+        <v>799</v>
+      </c>
+      <c r="D161" s="43" t="s">
         <v>801</v>
-      </c>
-      <c r="D161" s="43" t="s">
-        <v>803</v>
       </c>
       <c r="E161" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F161" s="37" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="G161" s="93" t="s">
         <v>338</v>
@@ -27849,7 +27850,7 @@
         <v>340</v>
       </c>
       <c r="I161" s="26" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="J161" s="48" t="s">
         <v>391</v>
@@ -27866,16 +27867,16 @@
         <v>441</v>
       </c>
       <c r="C162" s="94" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="D162" s="43" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="E162" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F162" s="37" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="G162" s="93" t="s">
         <v>338</v>
@@ -27884,7 +27885,7 @@
         <v>340</v>
       </c>
       <c r="I162" s="26" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="J162" s="48" t="s">
         <v>391</v>
@@ -27901,16 +27902,16 @@
         <v>364</v>
       </c>
       <c r="C163" s="94" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D163" s="43" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="E163" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F163" s="37" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="G163" s="93" t="s">
         <v>333</v>
@@ -27919,7 +27920,7 @@
         <v>340</v>
       </c>
       <c r="I163" s="30" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="J163" s="48" t="s">
         <v>395</v>
@@ -27936,16 +27937,16 @@
         <v>364</v>
       </c>
       <c r="C164" s="94" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D164" s="43" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="E164" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F164" s="37" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="G164" s="93" t="s">
         <v>333</v>
@@ -27954,7 +27955,7 @@
         <v>340</v>
       </c>
       <c r="I164" s="30" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="J164" s="48" t="s">
         <v>395</v>
@@ -27971,16 +27972,16 @@
         <v>364</v>
       </c>
       <c r="C165" s="94" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D165" s="43" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="E165" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F165" s="37" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="G165" s="93" t="s">
         <v>333</v>
@@ -27989,7 +27990,7 @@
         <v>340</v>
       </c>
       <c r="I165" s="30" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="J165" s="48" t="s">
         <v>395</v>
@@ -28006,16 +28007,16 @@
         <v>364</v>
       </c>
       <c r="C166" s="94" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="D166" s="93" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="E166" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F166" s="37" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="G166" s="93" t="s">
         <v>333</v>
@@ -28024,7 +28025,7 @@
         <v>340</v>
       </c>
       <c r="I166" s="30" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="J166" s="48" t="s">
         <v>395</v>
@@ -28038,19 +28039,19 @@
         <v>91</v>
       </c>
       <c r="B167" s="53" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="C167" s="94" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="D167" s="93" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="E167" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F167" s="37" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="G167" s="93" t="s">
         <v>338</v>
@@ -28059,13 +28060,13 @@
         <v>340</v>
       </c>
       <c r="I167" s="30" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="J167" s="48" t="s">
         <v>391</v>
       </c>
       <c r="K167" s="48" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="168" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -28345,7 +28346,7 @@
         <v>536</v>
       </c>
       <c r="G186" s="55" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="H186" s="55"/>
       <c r="I186" s="55"/>
@@ -28354,13 +28355,13 @@
     <row r="187" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B187" s="53"/>
       <c r="C187" s="31" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D187" s="43" t="s">
         <v>514</v>
       </c>
       <c r="E187" s="55" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="F187" s="55"/>
       <c r="G187" s="55"/>
@@ -28371,13 +28372,13 @@
     <row r="188" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B188" s="53"/>
       <c r="C188" s="31" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D188" s="43" t="s">
         <v>514</v>
       </c>
       <c r="E188" s="55" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="F188" s="55"/>
       <c r="G188" s="55"/>
@@ -28388,14 +28389,14 @@
     <row r="189" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B189" s="53"/>
       <c r="C189" s="31" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D189" s="43" t="s">
         <v>513</v>
       </c>
       <c r="E189" s="55"/>
       <c r="F189" s="55" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="G189" s="55"/>
       <c r="H189" s="55"/>
@@ -28405,14 +28406,14 @@
     <row r="190" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B190" s="53"/>
       <c r="C190" s="31" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D190" s="43" t="s">
         <v>513</v>
       </c>
       <c r="E190" s="55"/>
       <c r="F190" s="55" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="G190" s="55"/>
       <c r="H190" s="55"/>
@@ -28422,7 +28423,7 @@
     <row r="191" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B191" s="53"/>
       <c r="C191" s="31" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="D191" s="43" t="s">
         <v>513</v>
@@ -28437,7 +28438,7 @@
     <row r="192" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B192" s="53"/>
       <c r="C192" s="31" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D192" s="43" t="s">
         <v>513</v>
@@ -28452,7 +28453,7 @@
     <row r="193" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B193" s="53"/>
       <c r="C193" s="31" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="D193" s="43" t="s">
         <v>513</v>
@@ -39313,7 +39314,7 @@
   <dimension ref="A2:Q210"/>
   <sheetViews>
     <sheetView topLeftCell="A69" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F85" sqref="F85"/>
+      <selection activeCell="C112" sqref="C112:I114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -39379,7 +39380,7 @@
         <v>259</v>
       </c>
       <c r="D6" s="95" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.45">
@@ -39736,7 +39737,7 @@
         <v>302</v>
       </c>
       <c r="G27" s="93" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="H27" s="34" t="s">
         <v>81</v>
@@ -39759,7 +39760,7 @@
         <v>85</v>
       </c>
       <c r="G28" s="93" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="H28" s="34" t="s">
         <v>88</v>
@@ -39782,7 +39783,7 @@
         <v>307</v>
       </c>
       <c r="G29" s="93" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="H29" s="34" t="s">
         <v>95</v>
@@ -39865,7 +39866,7 @@
         <v>117</v>
       </c>
       <c r="D33" s="93" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E33" s="93" t="s">
         <v>87</v>
@@ -39874,7 +39875,7 @@
         <v>316</v>
       </c>
       <c r="G33" s="93" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="H33" s="34" t="s">
         <v>119</v>
@@ -39989,7 +39990,7 @@
         <v>326</v>
       </c>
       <c r="G38" s="93" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="H38" s="34" t="s">
         <v>146</v>
@@ -40207,94 +40208,94 @@
     </row>
     <row r="48" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C48" s="33" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D48" s="93" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="E48" s="93" t="s">
         <v>87</v>
       </c>
       <c r="F48" s="93" t="s">
+        <v>685</v>
+      </c>
+      <c r="G48" s="93" t="s">
+        <v>736</v>
+      </c>
+      <c r="H48" s="34" t="s">
+        <v>686</v>
+      </c>
+      <c r="I48" s="93" t="s">
         <v>687</v>
-      </c>
-      <c r="G48" s="93" t="s">
-        <v>738</v>
-      </c>
-      <c r="H48" s="34" t="s">
-        <v>688</v>
-      </c>
-      <c r="I48" s="93" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C49" s="33" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="D49" s="93" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="E49" s="93" t="s">
         <v>87</v>
       </c>
       <c r="F49" s="93" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G49" s="93" t="s">
         <v>285</v>
       </c>
       <c r="H49" s="34" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="I49" s="93" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C50" s="33" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="D50" s="93" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="E50" s="93" t="s">
         <v>87</v>
       </c>
       <c r="F50" s="93" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G50" s="93" t="s">
         <v>285</v>
       </c>
       <c r="H50" s="34" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="I50" s="93" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.45">
       <c r="C51" s="33" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="D51" s="93" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="E51" s="93" t="s">
         <v>162</v>
       </c>
       <c r="F51" s="93" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="G51" s="93" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="H51" s="34" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="I51" s="93" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.45">
@@ -40638,7 +40639,7 @@
         <v>340</v>
       </c>
       <c r="I77" s="48" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="J77" t="s">
         <v>391</v>
@@ -40673,7 +40674,7 @@
         <v>340</v>
       </c>
       <c r="I78" s="48" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="J78" t="s">
         <v>391</v>
@@ -40761,16 +40762,16 @@
         <v>364</v>
       </c>
       <c r="C81" s="94" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="D81" s="93" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="E81" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F81" s="37" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="G81" s="93" t="s">
         <v>410</v>
@@ -40779,7 +40780,7 @@
         <v>340</v>
       </c>
       <c r="I81" s="30" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="J81" s="48" t="s">
         <v>395</v>
@@ -40795,16 +40796,16 @@
         <v>364</v>
       </c>
       <c r="C82" s="94" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="D82" s="93" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="E82" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F82" s="37" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="G82" s="93" t="s">
         <v>410</v>
@@ -40813,7 +40814,7 @@
         <v>340</v>
       </c>
       <c r="I82" s="30" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="J82" s="48" t="s">
         <v>395</v>
@@ -40829,16 +40830,16 @@
         <v>364</v>
       </c>
       <c r="C83" s="94" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="D83" s="93" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E83" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F83" s="37" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="G83" s="93" t="s">
         <v>338</v>
@@ -40847,7 +40848,7 @@
         <v>340</v>
       </c>
       <c r="I83" s="30" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="J83" s="48" t="s">
         <v>395</v>
@@ -40863,13 +40864,13 @@
         <v>364</v>
       </c>
       <c r="C84" s="94" t="s">
+        <v>803</v>
+      </c>
+      <c r="D84" s="93" t="s">
         <v>805</v>
       </c>
-      <c r="D84" s="93" t="s">
-        <v>807</v>
-      </c>
       <c r="E84" s="93" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="F84" s="37" t="s">
         <v>41</v>
@@ -40881,7 +40882,7 @@
         <v>340</v>
       </c>
       <c r="I84" s="30" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="J84" s="48" t="s">
         <v>395</v>
@@ -40917,7 +40918,7 @@
         <v>340</v>
       </c>
       <c r="I85" s="30" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="J85" t="s">
         <v>388</v>
@@ -41057,7 +41058,7 @@
         <v>340</v>
       </c>
       <c r="I89" s="50" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="J89" s="50" t="s">
         <v>388</v>
@@ -41096,7 +41097,7 @@
         <v>340</v>
       </c>
       <c r="I90" s="48" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="J90" s="50" t="s">
         <v>388</v>
@@ -41209,7 +41210,7 @@
         <v>340</v>
       </c>
       <c r="I93" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="J93" t="s">
         <v>391</v>
@@ -41350,7 +41351,7 @@
         <v>340</v>
       </c>
       <c r="I97" s="48" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="J97" t="s">
         <v>391</v>
@@ -41402,10 +41403,10 @@
         <v>364</v>
       </c>
       <c r="C99" s="94" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="D99" s="93" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="E99" s="93" t="s">
         <v>55</v>
@@ -41420,7 +41421,7 @@
         <v>340</v>
       </c>
       <c r="I99" s="48" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="J99" s="48" t="s">
         <v>391</v>
@@ -41437,10 +41438,10 @@
         <v>364</v>
       </c>
       <c r="C100" s="94" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="D100" s="93" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="E100" s="93" t="s">
         <v>55</v>
@@ -41455,7 +41456,7 @@
         <v>340</v>
       </c>
       <c r="I100" s="48" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="J100" s="48" t="s">
         <v>391</v>
@@ -41472,16 +41473,16 @@
         <v>364</v>
       </c>
       <c r="C101" s="94" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="D101" s="93" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="E101" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F101" s="37" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="G101" s="93" t="s">
         <v>333</v>
@@ -41490,7 +41491,7 @@
         <v>340</v>
       </c>
       <c r="I101" s="48" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="J101" s="48" t="s">
         <v>391</v>
@@ -41564,7 +41565,7 @@
         <v>340</v>
       </c>
       <c r="I103" s="50" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="J103" s="50" t="s">
         <v>391</v>
@@ -41624,16 +41625,16 @@
         <v>364</v>
       </c>
       <c r="C105" s="94" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="D105" s="98" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="E105" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F105" s="41" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="G105" s="93" t="s">
         <v>338</v>
@@ -41642,7 +41643,7 @@
         <v>340</v>
       </c>
       <c r="I105" s="48" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="J105" s="50" t="s">
         <v>391</v>
@@ -41663,16 +41664,16 @@
         <v>364</v>
       </c>
       <c r="C106" s="94" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="D106" s="98" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E106" s="93" t="s">
         <v>28</v>
       </c>
       <c r="F106" s="41" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="G106" s="93" t="s">
         <v>338</v>
@@ -41681,7 +41682,7 @@
         <v>340</v>
       </c>
       <c r="I106" s="48" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="J106" s="50" t="s">
         <v>391</v>
@@ -41700,16 +41701,16 @@
         <v>364</v>
       </c>
       <c r="C107" s="94" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="D107" s="98" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="E107" s="93" t="s">
         <v>28</v>
       </c>
       <c r="F107" s="41" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="G107" s="93" t="s">
         <v>333</v>
@@ -41718,7 +41719,7 @@
         <v>340</v>
       </c>
       <c r="I107" s="26" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="J107" s="50" t="s">
         <v>391</v>
@@ -41755,7 +41756,7 @@
         <v>340</v>
       </c>
       <c r="I108" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="J108" t="s">
         <v>391</v>
@@ -41790,7 +41791,7 @@
         <v>340</v>
       </c>
       <c r="I109" s="48" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="J109" t="s">
         <v>391</v>
@@ -41886,7 +41887,7 @@
         <v>431</v>
       </c>
       <c r="E112" s="93" t="s">
-        <v>595</v>
+        <v>806</v>
       </c>
       <c r="F112" s="39" t="s">
         <v>137</v>
@@ -41897,8 +41898,8 @@
       <c r="H112" s="93" t="s">
         <v>340</v>
       </c>
-      <c r="I112" s="96" t="s">
-        <v>596</v>
+      <c r="I112" s="50" t="s">
+        <v>807</v>
       </c>
       <c r="J112" t="s">
         <v>395</v>
@@ -41921,7 +41922,7 @@
         <v>433</v>
       </c>
       <c r="E113" s="93" t="s">
-        <v>97</v>
+        <v>595</v>
       </c>
       <c r="F113" s="37" t="s">
         <v>143</v>
@@ -41932,8 +41933,8 @@
       <c r="H113" s="93" t="s">
         <v>340</v>
       </c>
-      <c r="I113" t="s">
-        <v>434</v>
+      <c r="I113" s="50" t="s">
+        <v>808</v>
       </c>
       <c r="J113" t="s">
         <v>395</v>
@@ -41956,7 +41957,7 @@
         <v>435</v>
       </c>
       <c r="E114" s="93" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="F114" s="37" t="s">
         <v>148</v>
@@ -41967,8 +41968,8 @@
       <c r="H114" s="93" t="s">
         <v>340</v>
       </c>
-      <c r="I114" t="s">
-        <v>597</v>
+      <c r="I114" s="50" t="s">
+        <v>809</v>
       </c>
       <c r="J114" t="s">
         <v>395</v>
@@ -42073,7 +42074,7 @@
         <v>340</v>
       </c>
       <c r="I117" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="J117" t="s">
         <v>391</v>
@@ -42096,7 +42097,7 @@
         <v>445</v>
       </c>
       <c r="E118" s="93" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="F118" s="37" t="s">
         <v>172</v>
@@ -42108,7 +42109,7 @@
         <v>340</v>
       </c>
       <c r="I118" s="48" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="J118" t="s">
         <v>391</v>
@@ -42143,7 +42144,7 @@
         <v>340</v>
       </c>
       <c r="I119" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="J119" t="s">
         <v>391</v>
@@ -42285,7 +42286,7 @@
         <v>340</v>
       </c>
       <c r="I123" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="J123" s="55" t="s">
         <v>457</v>
@@ -42374,16 +42375,16 @@
         <v>364</v>
       </c>
       <c r="C126" s="94" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D126" s="93" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="E126" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F126" s="37" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="G126" s="93" t="s">
         <v>338</v>
@@ -42392,7 +42393,7 @@
         <v>340</v>
       </c>
       <c r="I126" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="J126" s="55" t="s">
         <v>457</v>
@@ -42485,10 +42486,10 @@
         <v>206</v>
       </c>
       <c r="D129" s="93" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E129" s="93" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="F129" s="37" t="s">
         <v>207</v>
@@ -42500,7 +42501,7 @@
         <v>340</v>
       </c>
       <c r="I129" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="J129" s="55" t="s">
         <v>457</v>
@@ -42521,7 +42522,7 @@
         <v>208</v>
       </c>
       <c r="D130" s="93" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="E130" s="93" t="s">
         <v>40</v>
@@ -42554,16 +42555,16 @@
         <v>444</v>
       </c>
       <c r="C131" s="94" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D131" s="93" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="E131" s="93" t="s">
         <v>28</v>
       </c>
       <c r="F131" s="37" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="G131" s="93" t="s">
         <v>333</v>
@@ -42572,7 +42573,7 @@
         <v>340</v>
       </c>
       <c r="I131" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="J131" s="55" t="s">
         <v>457</v>
@@ -42608,7 +42609,7 @@
         <v>340</v>
       </c>
       <c r="I132" s="48" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="J132" t="s">
         <v>391</v>
@@ -42715,7 +42716,7 @@
         <v>340</v>
       </c>
       <c r="I135" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="J135" t="s">
         <v>395</v>
@@ -42750,7 +42751,7 @@
         <v>340</v>
       </c>
       <c r="I136" s="30" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="J136" t="s">
         <v>395</v>
@@ -42767,7 +42768,7 @@
         <v>364</v>
       </c>
       <c r="C137" s="94" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D137" s="95" t="s">
         <v>475</v>
@@ -42776,7 +42777,7 @@
         <v>55</v>
       </c>
       <c r="F137" s="37" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="G137" s="93" t="s">
         <v>386</v>
@@ -42785,7 +42786,7 @@
         <v>340</v>
       </c>
       <c r="I137" s="30" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="J137" t="s">
         <v>395</v>
@@ -42840,7 +42841,7 @@
         <v>222</v>
       </c>
       <c r="D139" s="95" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="E139" s="93" t="s">
         <v>238</v>
@@ -42855,7 +42856,7 @@
         <v>340</v>
       </c>
       <c r="I139" s="48" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="J139" t="s">
         <v>395</v>
@@ -42872,10 +42873,10 @@
         <v>364</v>
       </c>
       <c r="C140" s="94" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D140" s="95" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E140" s="93" t="s">
         <v>55</v>
@@ -42890,7 +42891,7 @@
         <v>340</v>
       </c>
       <c r="I140" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J140" t="s">
         <v>395</v>
@@ -42960,7 +42961,7 @@
         <v>340</v>
       </c>
       <c r="I142" s="48" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="J142" t="s">
         <v>395</v>
@@ -42977,10 +42978,10 @@
         <v>364</v>
       </c>
       <c r="C143" s="94" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D143" s="93" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="E143" s="93" t="s">
         <v>55</v>
@@ -42995,7 +42996,7 @@
         <v>340</v>
       </c>
       <c r="I143" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="J143" t="s">
         <v>395</v>
@@ -43065,7 +43066,7 @@
         <v>340</v>
       </c>
       <c r="I145" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="J145" t="s">
         <v>395</v>
@@ -43082,10 +43083,10 @@
         <v>364</v>
       </c>
       <c r="C146" s="94" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D146" s="93" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="E146" s="93" t="s">
         <v>55</v>
@@ -43100,7 +43101,7 @@
         <v>340</v>
       </c>
       <c r="I146" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="J146" t="s">
         <v>395</v>
@@ -43170,7 +43171,7 @@
         <v>340</v>
       </c>
       <c r="I148" s="30" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="J148" t="s">
         <v>395</v>
@@ -43258,10 +43259,10 @@
         <v>364</v>
       </c>
       <c r="C151" s="94" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D151" s="42" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="E151" s="93" t="s">
         <v>55</v>
@@ -43276,7 +43277,7 @@
         <v>340</v>
       </c>
       <c r="I151" s="97" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="J151" t="s">
         <v>395</v>
@@ -43293,10 +43294,10 @@
         <v>364</v>
       </c>
       <c r="C152" s="94" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D152" s="42" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E152" s="93" t="s">
         <v>55</v>
@@ -43311,7 +43312,7 @@
         <v>340</v>
       </c>
       <c r="I152" s="30" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="J152" t="s">
         <v>395</v>
@@ -43334,7 +43335,7 @@
         <v>498</v>
       </c>
       <c r="E153" s="93" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="F153" s="37" t="s">
         <v>247</v>
@@ -43346,7 +43347,7 @@
         <v>340</v>
       </c>
       <c r="I153" s="48" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="J153" t="s">
         <v>391</v>
@@ -43468,16 +43469,16 @@
         <v>444</v>
       </c>
       <c r="C157" s="94" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="D157" s="43" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="E157" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F157" s="37" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="G157" s="93" t="s">
         <v>333</v>
@@ -43486,13 +43487,13 @@
         <v>340</v>
       </c>
       <c r="I157" s="48" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="J157" s="48" t="s">
         <v>391</v>
       </c>
       <c r="K157" s="55" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.45">
@@ -43500,13 +43501,13 @@
         <v>82</v>
       </c>
       <c r="B158" s="53" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C158" s="94" t="s">
+        <v>776</v>
+      </c>
+      <c r="D158" s="43" t="s">
         <v>778</v>
-      </c>
-      <c r="D158" s="43" t="s">
-        <v>780</v>
       </c>
       <c r="E158" s="93" t="s">
         <v>55</v>
@@ -43521,10 +43522,10 @@
         <v>340</v>
       </c>
       <c r="I158" s="48" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="J158" s="48" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="K158" s="55" t="s">
         <v>92</v>
@@ -43535,13 +43536,13 @@
         <v>83</v>
       </c>
       <c r="B159" s="53" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="C159" s="94" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="D159" s="43" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="E159" s="93" t="s">
         <v>55</v>
@@ -43556,10 +43557,10 @@
         <v>340</v>
       </c>
       <c r="I159" s="48" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="J159" s="48" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="K159" s="55" t="s">
         <v>92</v>
@@ -43573,16 +43574,16 @@
         <v>444</v>
       </c>
       <c r="C160" s="94" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="D160" s="43" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="E160" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F160" s="37" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="G160" s="93" t="s">
         <v>338</v>
@@ -43591,7 +43592,7 @@
         <v>340</v>
       </c>
       <c r="I160" s="26" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="J160" s="48" t="s">
         <v>391</v>
@@ -43608,16 +43609,16 @@
         <v>430</v>
       </c>
       <c r="C161" s="94" t="s">
+        <v>799</v>
+      </c>
+      <c r="D161" s="43" t="s">
         <v>801</v>
-      </c>
-      <c r="D161" s="43" t="s">
-        <v>803</v>
       </c>
       <c r="E161" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F161" s="37" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="G161" s="93" t="s">
         <v>338</v>
@@ -43626,7 +43627,7 @@
         <v>340</v>
       </c>
       <c r="I161" s="26" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="J161" s="48" t="s">
         <v>391</v>
@@ -43643,16 +43644,16 @@
         <v>441</v>
       </c>
       <c r="C162" s="94" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="D162" s="43" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="E162" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F162" s="37" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="G162" s="93" t="s">
         <v>338</v>
@@ -43661,7 +43662,7 @@
         <v>340</v>
       </c>
       <c r="I162" s="26" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="J162" s="48" t="s">
         <v>391</v>
@@ -43678,16 +43679,16 @@
         <v>364</v>
       </c>
       <c r="C163" s="94" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D163" s="43" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="E163" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F163" s="37" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="G163" s="93" t="s">
         <v>333</v>
@@ -43696,7 +43697,7 @@
         <v>340</v>
       </c>
       <c r="I163" s="30" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="J163" s="48" t="s">
         <v>395</v>
@@ -43713,16 +43714,16 @@
         <v>364</v>
       </c>
       <c r="C164" s="94" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D164" s="43" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="E164" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F164" s="37" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="G164" s="93" t="s">
         <v>333</v>
@@ -43731,7 +43732,7 @@
         <v>340</v>
       </c>
       <c r="I164" s="30" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="J164" s="48" t="s">
         <v>395</v>
@@ -43748,16 +43749,16 @@
         <v>364</v>
       </c>
       <c r="C165" s="94" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D165" s="43" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="E165" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F165" s="37" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="G165" s="93" t="s">
         <v>333</v>
@@ -43766,7 +43767,7 @@
         <v>340</v>
       </c>
       <c r="I165" s="30" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="J165" s="48" t="s">
         <v>395</v>
@@ -43783,16 +43784,16 @@
         <v>364</v>
       </c>
       <c r="C166" s="94" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="D166" s="93" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="E166" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F166" s="37" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="G166" s="93" t="s">
         <v>333</v>
@@ -43801,7 +43802,7 @@
         <v>340</v>
       </c>
       <c r="I166" s="30" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="J166" s="48" t="s">
         <v>395</v>
@@ -43815,19 +43816,19 @@
         <v>91</v>
       </c>
       <c r="B167" s="53" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="C167" s="94" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="D167" s="93" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="E167" s="93" t="s">
         <v>55</v>
       </c>
       <c r="F167" s="37" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="G167" s="93" t="s">
         <v>338</v>
@@ -43836,13 +43837,13 @@
         <v>340</v>
       </c>
       <c r="I167" s="30" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="J167" s="48" t="s">
         <v>391</v>
       </c>
       <c r="K167" s="48" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
     </row>
     <row r="168" spans="1:14" ht="15.6" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -44113,7 +44114,7 @@
         <v>534</v>
       </c>
       <c r="D186" s="43" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="E186" s="55" t="s">
         <v>535</v>
@@ -44122,7 +44123,7 @@
         <v>536</v>
       </c>
       <c r="G186" s="55" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="H186" s="55"/>
       <c r="I186" s="55"/>
@@ -44131,13 +44132,13 @@
     <row r="187" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B187" s="53"/>
       <c r="C187" s="31" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D187" s="43" t="s">
         <v>514</v>
       </c>
       <c r="E187" s="55" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="F187" s="55"/>
       <c r="G187" s="55"/>
@@ -44148,13 +44149,13 @@
     <row r="188" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B188" s="53"/>
       <c r="C188" s="31" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="D188" s="43" t="s">
         <v>514</v>
       </c>
       <c r="E188" s="55" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="F188" s="55"/>
       <c r="G188" s="55"/>
@@ -44165,14 +44166,14 @@
     <row r="189" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B189" s="53"/>
       <c r="C189" s="31" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="D189" s="43" t="s">
         <v>513</v>
       </c>
       <c r="E189" s="55"/>
       <c r="F189" s="55" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="G189" s="55"/>
       <c r="H189" s="55"/>
@@ -44182,14 +44183,14 @@
     <row r="190" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B190" s="53"/>
       <c r="C190" s="31" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="D190" s="43" t="s">
         <v>513</v>
       </c>
       <c r="E190" s="55"/>
       <c r="F190" s="55" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="G190" s="55"/>
       <c r="H190" s="55"/>
@@ -44199,7 +44200,7 @@
     <row r="191" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B191" s="53"/>
       <c r="C191" s="31" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="D191" s="43" t="s">
         <v>513</v>
@@ -44214,7 +44215,7 @@
     <row r="192" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B192" s="53"/>
       <c r="C192" s="31" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="D192" s="43" t="s">
         <v>513</v>
@@ -44229,7 +44230,7 @@
     <row r="193" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B193" s="53"/>
       <c r="C193" s="31" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="D193" s="43" t="s">
         <v>513</v>
@@ -44425,7 +44426,7 @@
         <v>256</v>
       </c>
       <c r="D4" s="95" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.45">
@@ -44433,7 +44434,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="95" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.45">
@@ -44449,7 +44450,7 @@
         <v>261</v>
       </c>
       <c r="D7" s="93" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="E7" t="s">
         <v>263</v>
@@ -44659,7 +44660,7 @@
         <v>287</v>
       </c>
       <c r="G21" s="93" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="H21" s="34" t="s">
         <v>47</v>
@@ -48003,7 +48004,7 @@
         <v>256</v>
       </c>
       <c r="D4" s="95" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.45">
@@ -48011,7 +48012,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="95" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.45">
@@ -48027,7 +48028,7 @@
         <v>261</v>
       </c>
       <c r="D7" s="93" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="E7" t="s">
         <v>263</v>
@@ -48237,7 +48238,7 @@
         <v>287</v>
       </c>
       <c r="G21" s="93" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="H21" s="34" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Included pav in dyn. material composition calculation.
</commit_message>
<xml_diff>
--- a/RECC_Config_V2_4.xlsx
+++ b/RECC_Config_V2_4.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10272" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10272" uniqueCount="803">
   <si>
     <t>User Name</t>
   </si>
@@ -2434,6 +2434,9 @@
   </si>
   <si>
     <t>8e82f0fc-9028-46d8-b3ab-126552690928</t>
+  </si>
+  <si>
+    <t>[0,2,4,6,7]</t>
   </si>
 </sst>
 </file>
@@ -10941,8 +10944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11378,7 +11381,7 @@
         <v>303</v>
       </c>
       <c r="G27" s="96" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="H27" s="34" t="s">
         <v>80</v>
@@ -11410,7 +11413,7 @@
         <v>84</v>
       </c>
       <c r="G28" s="96" t="s">
-        <v>308</v>
+        <v>802</v>
       </c>
       <c r="H28" s="34" t="s">
         <v>87</v>
@@ -11442,7 +11445,7 @@
         <v>312</v>
       </c>
       <c r="G29" s="96" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="H29" s="34" t="s">
         <v>94</v>
@@ -15867,7 +15870,7 @@
         <v>712</v>
       </c>
       <c r="D181" s="96" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E181" t="s">
         <v>714</v>
@@ -15882,7 +15885,7 @@
         <v>715</v>
       </c>
       <c r="D182" s="96" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E182" t="s">
         <v>714</v>
@@ -15897,7 +15900,7 @@
         <v>716</v>
       </c>
       <c r="D183" s="96" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E183" s="55" t="s">
         <v>714</v>
@@ -15948,7 +15951,7 @@
         <v>721</v>
       </c>
       <c r="D186" s="96" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E186" s="55" t="s">
         <v>714</v>
@@ -15966,7 +15969,7 @@
         <v>723</v>
       </c>
       <c r="D187" s="96" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E187" t="s">
         <v>714</v>
@@ -15981,7 +15984,7 @@
         <v>724</v>
       </c>
       <c r="D188" s="96" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E188" t="s">
         <v>714</v>
@@ -15996,7 +15999,7 @@
         <v>725</v>
       </c>
       <c r="D189" s="96" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E189" s="55" t="s">
         <v>714</v>
@@ -16011,7 +16014,7 @@
         <v>726</v>
       </c>
       <c r="D190" s="96" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E190" s="55" t="s">
         <v>714</v>
@@ -16029,7 +16032,7 @@
         <v>728</v>
       </c>
       <c r="D191" s="96" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E191" s="55" t="s">
         <v>714</v>
@@ -16047,7 +16050,7 @@
         <v>730</v>
       </c>
       <c r="D192" s="96" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E192" s="55" t="s">
         <v>714</v>
@@ -16065,7 +16068,7 @@
         <v>731</v>
       </c>
       <c r="D193" s="96" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E193" s="55" t="s">
         <v>714</v>
@@ -16083,7 +16086,7 @@
         <v>732</v>
       </c>
       <c r="D194" s="96" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="E194" s="55" t="s">
         <v>714</v>
@@ -16100,7 +16103,7 @@
         <v>734</v>
       </c>
       <c r="D195" s="43" t="s">
-        <v>735</v>
+        <v>743</v>
       </c>
       <c r="E195" s="55" t="s">
         <v>736</v>

</xml_diff>

<commit_message>
Fixed process number for S12 and dS12 (12 instead of 10) so that the mass bal. for NoScrapExport option works correctly.
</commit_message>
<xml_diff>
--- a/RECC_Config_V2_4.xlsx
+++ b/RECC_Config_V2_4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9405" windowWidth="20730" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9405" windowWidth="20730" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cover" sheetId="1" state="visible" r:id="rId1"/>
@@ -1485,8 +1485,8 @@
     <col bestFit="1" customWidth="1" max="9" min="9" style="53" width="8.265625"/>
     <col customWidth="1" max="10" min="10" style="55" width="39.86328125"/>
     <col customWidth="1" max="11" min="11" style="53" width="46.73046875"/>
-    <col customWidth="1" max="49" min="12" style="53" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="50" style="53" width="10.6640625"/>
+    <col customWidth="1" max="52" min="12" style="53" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="53" style="53" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="8">
@@ -1886,7 +1886,7 @@
   </sheetPr>
   <dimension ref="A2:Q221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B100" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+    <sheetView topLeftCell="B100" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
       <selection activeCell="E126" sqref="E126:I126"/>
     </sheetView>
   </sheetViews>
@@ -1906,8 +1906,8 @@
     <col customWidth="1" max="12" min="12" style="69" width="15.53125"/>
     <col customWidth="1" max="13" min="13" style="69" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="69" width="90"/>
-    <col customWidth="1" max="88" min="15" style="69" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="89" style="69" width="10.6640625"/>
+    <col customWidth="1" max="91" min="15" style="69" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="92" style="69" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -10085,8 +10085,8 @@
   </sheetPr>
   <dimension ref="A2:Q221"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="E132" sqref="E132"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="D186" sqref="D186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -10105,8 +10105,8 @@
     <col customWidth="1" max="12" min="12" style="69" width="15.53125"/>
     <col customWidth="1" max="13" min="13" style="69" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="69" width="90"/>
-    <col customWidth="1" max="88" min="15" style="69" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="89" style="69" width="10.6640625"/>
+    <col customWidth="1" max="91" min="15" style="69" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="92" style="69" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -10182,7 +10182,7 @@
       </c>
       <c r="D7" s="63" t="inlineStr">
         <is>
-          <t>Germany_detail</t>
+          <t>Global_all</t>
         </is>
       </c>
     </row>
@@ -10494,7 +10494,7 @@
       </c>
       <c r="G21" s="63" t="inlineStr">
         <is>
-          <t>[33]</t>
+          <t>[2,13,31,32,33,34,35,36,37,38,39,9,4,12,40,41,42,43,44,45]</t>
         </is>
       </c>
       <c r="H21" s="33" t="inlineStr">
@@ -10717,7 +10717,7 @@
       </c>
       <c r="G27" s="63" t="inlineStr">
         <is>
-          <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58]</t>
+          <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34,59,60,61,62,76,77,78,79,80,81,82,83,84,85,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105]</t>
         </is>
       </c>
       <c r="H27" s="33" t="inlineStr">
@@ -10754,7 +10754,7 @@
       </c>
       <c r="G28" s="63" t="inlineStr">
         <is>
-          <t>[0,2,3]</t>
+          <t>[0,2,4,6,7]</t>
         </is>
       </c>
       <c r="H28" s="33" t="inlineStr">
@@ -10791,7 +10791,7 @@
       </c>
       <c r="G29" s="63" t="inlineStr">
         <is>
-          <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58]</t>
+          <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34,59,60,61,62,76,77,78,79,80,81,82,83,84,85,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105]</t>
         </is>
       </c>
       <c r="H29" s="33" t="inlineStr">
@@ -10939,7 +10939,7 @@
       </c>
       <c r="G33" s="63" t="inlineStr">
         <is>
-          <t>[0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23]</t>
+          <t>[24,25,26,27]</t>
         </is>
       </c>
       <c r="H33" s="33" t="inlineStr">
@@ -11494,7 +11494,7 @@
       </c>
       <c r="G48" s="63" t="inlineStr">
         <is>
-          <t>all</t>
+          <t>[0:19)</t>
         </is>
       </c>
       <c r="H48" s="33" t="inlineStr">
@@ -17727,7 +17727,7 @@
       </c>
       <c r="D183" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="I183" s="56" t="n"/>
@@ -17740,7 +17740,7 @@
       </c>
       <c r="D184" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="I184" s="56" t="n"/>
@@ -17753,7 +17753,7 @@
       </c>
       <c r="D185" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E185" s="52" t="n"/>
@@ -17767,7 +17767,7 @@
       </c>
       <c r="D186" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E186" s="52" t="inlineStr">
@@ -17785,7 +17785,7 @@
       </c>
       <c r="D187" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E187" s="52" t="inlineStr">
@@ -17821,7 +17821,7 @@
       </c>
       <c r="D189" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="J189" s="50" t="n"/>
@@ -17834,7 +17834,7 @@
       </c>
       <c r="D190" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="J190" s="50" t="n"/>
@@ -17847,7 +17847,7 @@
       </c>
       <c r="D191" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E191" s="52" t="n"/>
@@ -17861,7 +17861,7 @@
       </c>
       <c r="D192" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E192" s="52" t="n"/>
@@ -17899,7 +17899,7 @@
       </c>
       <c r="D194" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E194" s="52" t="n"/>
@@ -17918,7 +17918,7 @@
       </c>
       <c r="D195" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E195" s="52" t="n"/>
@@ -17955,7 +17955,7 @@
       </c>
       <c r="D197" s="42" t="inlineStr">
         <is>
-          <t>['pav']</t>
+          <t>['pav','reb','nrbg','app','ind']</t>
         </is>
       </c>
       <c r="E197" s="52" t="n"/>
@@ -18284,8 +18284,8 @@
   </sheetPr>
   <dimension ref="A2:Q221"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
-      <selection activeCell="E126" sqref="E126:I126"/>
+    <sheetView workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -18304,8 +18304,8 @@
     <col customWidth="1" max="12" min="12" style="69" width="15.53125"/>
     <col customWidth="1" max="13" min="13" style="69" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="69" width="90"/>
-    <col customWidth="1" max="88" min="15" style="69" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="89" style="69" width="10.6640625"/>
+    <col customWidth="1" max="91" min="15" style="69" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="92" style="69" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -18693,7 +18693,7 @@
       </c>
       <c r="G21" s="63" t="inlineStr">
         <is>
-          <t>[2,13,31,32,33,34,35,36,37,38,39,9,4,12,40,41,42,43,44,45]</t>
+          <t>[2]</t>
         </is>
       </c>
       <c r="H21" s="33" t="inlineStr">
@@ -18914,9 +18914,10 @@
           <t>Manufacturing_i3</t>
         </is>
       </c>
-      <c r="G27" s="63">
-        <f>G29</f>
-        <v/>
+      <c r="G27" s="63" t="inlineStr">
+        <is>
+          <t>[0,1,2,3,4,5,59,60,61,62,76,77,78,79,80,81,82,83,84,85,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105]</t>
+        </is>
       </c>
       <c r="H27" s="33" t="inlineStr">
         <is>
@@ -18952,7 +18953,7 @@
       </c>
       <c r="G28" s="63" t="inlineStr">
         <is>
-          <t>[0,2,4,6,7]</t>
+          <t>[4,6,7]</t>
         </is>
       </c>
       <c r="H28" s="33" t="inlineStr">
@@ -18989,7 +18990,7 @@
       </c>
       <c r="G29" s="63" t="inlineStr">
         <is>
-          <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34,59,60,61,62,76,77,78,79,80,81,82,83,84,85,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105]</t>
+          <t>[0,1,2,3,4,5,59,60,61,62,76,77,78,79,80,81,82,83,84,85,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105]</t>
         </is>
       </c>
       <c r="H29" s="33" t="inlineStr">
@@ -19692,7 +19693,7 @@
       </c>
       <c r="G48" s="63" t="inlineStr">
         <is>
-          <t>[0:19)</t>
+          <t>[0:6)</t>
         </is>
       </c>
       <c r="H48" s="33" t="inlineStr">
@@ -25925,7 +25926,7 @@
       </c>
       <c r="D183" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="I183" s="56" t="n"/>
@@ -25938,7 +25939,7 @@
       </c>
       <c r="D184" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="I184" s="56" t="n"/>
@@ -25951,7 +25952,7 @@
       </c>
       <c r="D185" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E185" s="52" t="n"/>
@@ -26019,7 +26020,7 @@
       </c>
       <c r="D189" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="J189" s="50" t="n"/>
@@ -26032,7 +26033,7 @@
       </c>
       <c r="D190" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="J190" s="50" t="n"/>
@@ -26045,7 +26046,7 @@
       </c>
       <c r="D191" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E191" s="52" t="n"/>
@@ -26059,7 +26060,7 @@
       </c>
       <c r="D192" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E192" s="52" t="n"/>
@@ -26078,7 +26079,7 @@
       </c>
       <c r="D193" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E193" s="52" t="n"/>
@@ -26097,7 +26098,7 @@
       </c>
       <c r="D194" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E194" s="52" t="n"/>
@@ -26116,7 +26117,7 @@
       </c>
       <c r="D195" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E195" s="52" t="n"/>
@@ -26153,7 +26154,7 @@
       </c>
       <c r="D197" s="42" t="inlineStr">
         <is>
-          <t>['pav','reb']</t>
+          <t>['nrbg','app','ind']</t>
         </is>
       </c>
       <c r="E197" s="52" t="n"/>
@@ -26481,10 +26482,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B3:K30"/>
+  <dimension ref="B3:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -26520,6 +26521,11 @@
           <t>'pav','reb','nrb'</t>
         </is>
       </c>
+      <c r="G3" s="64" t="inlineStr">
+        <is>
+          <t>ind','nrbg','app'</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
@@ -26572,6 +26578,11 @@
       <c r="F5" t="inlineStr">
         <is>
           <t>[0,2,3]</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>[4,6,7]</t>
         </is>
       </c>
     </row>
@@ -26618,6 +26629,11 @@
       <c r="K8" s="63" t="inlineStr">
         <is>
           <t>RECC Germany detail</t>
+        </is>
+      </c>
+      <c r="L8" s="63" t="inlineStr">
+        <is>
+          <t>RECC global ind app nrbg</t>
         </is>
       </c>
     </row>
@@ -26647,6 +26663,7 @@
       <c r="I9" s="63" t="n"/>
       <c r="J9" s="63" t="n"/>
       <c r="K9" s="63" t="n"/>
+      <c r="L9" s="63" t="n"/>
     </row>
     <row r="10">
       <c r="B10" t="inlineStr">
@@ -26690,6 +26707,11 @@
           <t>[0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23]</t>
         </is>
       </c>
+      <c r="L10" s="63" t="inlineStr">
+        <is>
+          <t>[24,25,26,27]</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="B11" t="inlineStr">
@@ -26733,6 +26755,11 @@
           <t>all</t>
         </is>
       </c>
+      <c r="L11" s="63" t="inlineStr">
+        <is>
+          <t>[0:6)</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="B12" t="inlineStr">
@@ -26776,6 +26803,11 @@
           <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58]</t>
         </is>
       </c>
+      <c r="L12" s="63" t="inlineStr">
+        <is>
+          <t>[0,1,2,3,4,5,59,60,61,62,76,77,78,79,80,81,82,83,84,85,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105]</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="B13" t="inlineStr">
@@ -26819,6 +26851,11 @@
           <t>[0,2,3]</t>
         </is>
       </c>
+      <c r="L13" s="63" t="inlineStr">
+        <is>
+          <t>[4,6,7]</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="B14" t="inlineStr">
@@ -26860,6 +26897,11 @@
       <c r="K14" s="63" t="inlineStr">
         <is>
           <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58]</t>
+        </is>
+      </c>
+      <c r="L14" s="63" t="inlineStr">
+        <is>
+          <t>[0,1,2,3,4,5,59,60,61,62,76,77,78,79,80,81,82,83,84,85,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed nrb energy calculation to include post-2015 age-cohorts.
</commit_message>
<xml_diff>
--- a/RECC_Config_V2_4.xlsx
+++ b/RECC_Config_V2_4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9405" windowWidth="20730" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="4" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9405" windowWidth="20730" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cover" sheetId="1" state="visible" r:id="rId1"/>
@@ -1485,8 +1485,8 @@
     <col bestFit="1" customWidth="1" max="9" min="9" style="53" width="8.265625"/>
     <col customWidth="1" max="10" min="10" style="55" width="39.86328125"/>
     <col customWidth="1" max="11" min="11" style="53" width="46.73046875"/>
-    <col customWidth="1" max="52" min="12" style="53" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="53" style="53" width="10.6640625"/>
+    <col customWidth="1" max="53" min="12" style="53" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="54" style="53" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="8">
@@ -1886,8 +1886,8 @@
   </sheetPr>
   <dimension ref="A2:Q221"/>
   <sheetViews>
-    <sheetView topLeftCell="B100" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="E126" sqref="E126:I126"/>
+    <sheetView topLeftCell="C94" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1906,8 +1906,8 @@
     <col customWidth="1" max="12" min="12" style="69" width="15.53125"/>
     <col customWidth="1" max="13" min="13" style="69" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="69" width="90"/>
-    <col customWidth="1" max="91" min="15" style="69" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="92" style="69" width="10.6640625"/>
+    <col customWidth="1" max="92" min="15" style="69" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="93" style="69" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -5205,7 +5205,7 @@
       </c>
       <c r="E101" s="63" t="inlineStr">
         <is>
-          <t>V4.1</t>
+          <t>V4.2</t>
         </is>
       </c>
       <c r="F101" s="36" t="inlineStr">
@@ -5225,7 +5225,7 @@
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>6b281381-56a8-4761-a998-b3af0c4e2a80</t>
+          <t>3586fa40-404b-4f4b-afbb-ce76c5cf5402</t>
         </is>
       </c>
       <c r="J101" t="inlineStr">
@@ -10085,8 +10085,8 @@
   </sheetPr>
   <dimension ref="A2:Q221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="D186" sqref="D186"/>
+    <sheetView topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -10105,8 +10105,8 @@
     <col customWidth="1" max="12" min="12" style="69" width="15.53125"/>
     <col customWidth="1" max="13" min="13" style="69" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="69" width="90"/>
-    <col customWidth="1" max="91" min="15" style="69" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="92" style="69" width="10.6640625"/>
+    <col customWidth="1" max="92" min="15" style="69" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="93" style="69" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -10182,7 +10182,7 @@
       </c>
       <c r="D7" s="63" t="inlineStr">
         <is>
-          <t>Global_all</t>
+          <t>Germany_detail</t>
         </is>
       </c>
     </row>
@@ -10494,7 +10494,7 @@
       </c>
       <c r="G21" s="63" t="inlineStr">
         <is>
-          <t>[2,13,31,32,33,34,35,36,37,38,39,9,4,12,40,41,42,43,44,45]</t>
+          <t>[33]</t>
         </is>
       </c>
       <c r="H21" s="33" t="inlineStr">
@@ -10717,7 +10717,7 @@
       </c>
       <c r="G27" s="63" t="inlineStr">
         <is>
-          <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34,59,60,61,62,76,77,78,79,80,81,82,83,84,85,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105]</t>
+          <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58]</t>
         </is>
       </c>
       <c r="H27" s="33" t="inlineStr">
@@ -10754,7 +10754,7 @@
       </c>
       <c r="G28" s="63" t="inlineStr">
         <is>
-          <t>[0,2,4,6,7]</t>
+          <t>[0,2,3]</t>
         </is>
       </c>
       <c r="H28" s="33" t="inlineStr">
@@ -10791,7 +10791,7 @@
       </c>
       <c r="G29" s="63" t="inlineStr">
         <is>
-          <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34,59,60,61,62,76,77,78,79,80,81,82,83,84,85,86,87,88,89,90,91,92,93,94,95,96,97,98,99,100,101,102,103,104,105]</t>
+          <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58]</t>
         </is>
       </c>
       <c r="H29" s="33" t="inlineStr">
@@ -10939,7 +10939,7 @@
       </c>
       <c r="G33" s="63" t="inlineStr">
         <is>
-          <t>[24,25,26,27]</t>
+          <t>[0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23]</t>
         </is>
       </c>
       <c r="H33" s="33" t="inlineStr">
@@ -11494,7 +11494,7 @@
       </c>
       <c r="G48" s="63" t="inlineStr">
         <is>
-          <t>[0:19)</t>
+          <t>all</t>
         </is>
       </c>
       <c r="H48" s="33" t="inlineStr">
@@ -13405,7 +13405,7 @@
       </c>
       <c r="E101" s="63" t="inlineStr">
         <is>
-          <t>V4.1</t>
+          <t>V4.2</t>
         </is>
       </c>
       <c r="F101" s="36" t="inlineStr">
@@ -13425,7 +13425,7 @@
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>6b281381-56a8-4761-a998-b3af0c4e2a80</t>
+          <t>3586fa40-404b-4f4b-afbb-ce76c5cf5402</t>
         </is>
       </c>
       <c r="J101" t="inlineStr">
@@ -17727,7 +17727,7 @@
       </c>
       <c r="D183" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="I183" s="56" t="n"/>
@@ -17740,7 +17740,7 @@
       </c>
       <c r="D184" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="I184" s="56" t="n"/>
@@ -17753,7 +17753,7 @@
       </c>
       <c r="D185" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E185" s="52" t="n"/>
@@ -17767,7 +17767,7 @@
       </c>
       <c r="D186" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E186" s="52" t="inlineStr">
@@ -17785,7 +17785,7 @@
       </c>
       <c r="D187" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E187" s="52" t="inlineStr">
@@ -17821,7 +17821,7 @@
       </c>
       <c r="D189" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J189" s="50" t="n"/>
@@ -17834,7 +17834,7 @@
       </c>
       <c r="D190" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J190" s="50" t="n"/>
@@ -17847,7 +17847,7 @@
       </c>
       <c r="D191" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E191" s="52" t="n"/>
@@ -17861,7 +17861,7 @@
       </c>
       <c r="D192" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E192" s="52" t="n"/>
@@ -17880,7 +17880,7 @@
       </c>
       <c r="D193" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E193" s="52" t="n"/>
@@ -17955,7 +17955,7 @@
       </c>
       <c r="D197" s="42" t="inlineStr">
         <is>
-          <t>['pav','reb','nrbg','app','ind']</t>
+          <t>['nrb']</t>
         </is>
       </c>
       <c r="E197" s="52" t="n"/>
@@ -18284,8 +18284,8 @@
   </sheetPr>
   <dimension ref="A2:Q221"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
+      <selection activeCell="E101" sqref="E101:I101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -18304,8 +18304,8 @@
     <col customWidth="1" max="12" min="12" style="69" width="15.53125"/>
     <col customWidth="1" max="13" min="13" style="69" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="69" width="90"/>
-    <col customWidth="1" max="91" min="15" style="69" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="92" style="69" width="10.6640625"/>
+    <col customWidth="1" max="92" min="15" style="69" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="93" style="69" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -21604,7 +21604,7 @@
       </c>
       <c r="E101" s="63" t="inlineStr">
         <is>
-          <t>V4.1</t>
+          <t>V4.2</t>
         </is>
       </c>
       <c r="F101" s="36" t="inlineStr">
@@ -21624,7 +21624,7 @@
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>6b281381-56a8-4761-a998-b3af0c4e2a80</t>
+          <t>3586fa40-404b-4f4b-afbb-ce76c5cf5402</t>
         </is>
       </c>
       <c r="J101" t="inlineStr">

</xml_diff>

<commit_message>
added export of use phase energy flows and total energy (sum over carriers). ODYM-RECCv2.4 ready for final model run.
</commit_message>
<xml_diff>
--- a/RECC_Config_V2_4.xlsx
+++ b/RECC_Config_V2_4.xlsx
@@ -1485,8 +1485,8 @@
     <col bestFit="1" customWidth="1" max="9" min="9" style="53" width="8.265625"/>
     <col customWidth="1" max="10" min="10" style="55" width="39.86328125"/>
     <col customWidth="1" max="11" min="11" style="53" width="46.73046875"/>
-    <col customWidth="1" max="53" min="12" style="53" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="54" style="53" width="10.6640625"/>
+    <col customWidth="1" max="54" min="12" style="53" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="55" style="53" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="8">
@@ -1906,8 +1906,8 @@
     <col customWidth="1" max="12" min="12" style="69" width="15.53125"/>
     <col customWidth="1" max="13" min="13" style="69" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="69" width="90"/>
-    <col customWidth="1" max="92" min="15" style="69" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="93" style="69" width="10.6640625"/>
+    <col customWidth="1" max="93" min="15" style="69" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="94" style="69" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -10105,8 +10105,8 @@
     <col customWidth="1" max="12" min="12" style="69" width="15.53125"/>
     <col customWidth="1" max="13" min="13" style="69" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="69" width="90"/>
-    <col customWidth="1" max="92" min="15" style="69" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="93" style="69" width="10.6640625"/>
+    <col customWidth="1" max="93" min="15" style="69" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="94" style="69" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -17727,7 +17727,7 @@
       </c>
       <c r="D183" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="I183" s="56" t="n"/>
@@ -17740,7 +17740,7 @@
       </c>
       <c r="D184" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="I184" s="56" t="n"/>
@@ -17753,7 +17753,7 @@
       </c>
       <c r="D185" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E185" s="52" t="n"/>
@@ -17821,7 +17821,7 @@
       </c>
       <c r="D189" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="J189" s="50" t="n"/>
@@ -17834,7 +17834,7 @@
       </c>
       <c r="D190" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="J190" s="50" t="n"/>
@@ -17847,7 +17847,7 @@
       </c>
       <c r="D191" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E191" s="52" t="n"/>
@@ -17861,7 +17861,7 @@
       </c>
       <c r="D192" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E192" s="52" t="n"/>
@@ -17880,7 +17880,7 @@
       </c>
       <c r="D193" s="63" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>False</t>
         </is>
       </c>
       <c r="E193" s="52" t="n"/>
@@ -17955,7 +17955,7 @@
       </c>
       <c r="D197" s="42" t="inlineStr">
         <is>
-          <t>['nrb']</t>
+          <t>['pav']</t>
         </is>
       </c>
       <c r="E197" s="52" t="n"/>
@@ -18284,8 +18284,8 @@
   </sheetPr>
   <dimension ref="A2:Q221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
-      <selection activeCell="E101" sqref="E101:I101"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
+      <selection activeCell="F120" sqref="F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -18304,8 +18304,8 @@
     <col customWidth="1" max="12" min="12" style="69" width="15.53125"/>
     <col customWidth="1" max="13" min="13" style="69" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="69" width="90"/>
-    <col customWidth="1" max="92" min="15" style="69" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="93" style="69" width="10.6640625"/>
+    <col customWidth="1" max="93" min="15" style="69" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="94" style="69" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">

</xml_diff>

<commit_message>
added more plot options and svg export.
</commit_message>
<xml_diff>
--- a/RECC_Config_V2_4.xlsx
+++ b/RECC_Config_V2_4.xlsx
@@ -10182,7 +10182,7 @@
       </c>
       <c r="D7" s="63" t="inlineStr">
         <is>
-          <t>Germany_detail</t>
+          <t>R5.2REF_Other</t>
         </is>
       </c>
     </row>
@@ -10494,7 +10494,7 @@
       </c>
       <c r="G21" s="63" t="inlineStr">
         <is>
-          <t>[33]</t>
+          <t>[41]</t>
         </is>
       </c>
       <c r="H21" s="33" t="inlineStr">
@@ -10717,7 +10717,7 @@
       </c>
       <c r="G27" s="63" t="inlineStr">
         <is>
-          <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58]</t>
+          <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34]</t>
         </is>
       </c>
       <c r="H27" s="33" t="inlineStr">
@@ -10754,7 +10754,7 @@
       </c>
       <c r="G28" s="63" t="inlineStr">
         <is>
-          <t>[0,2,3]</t>
+          <t>[0,2]</t>
         </is>
       </c>
       <c r="H28" s="33" t="inlineStr">
@@ -10791,7 +10791,7 @@
       </c>
       <c r="G29" s="63" t="inlineStr">
         <is>
-          <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58]</t>
+          <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34]</t>
         </is>
       </c>
       <c r="H29" s="33" t="inlineStr">
@@ -10939,7 +10939,7 @@
       </c>
       <c r="G33" s="63" t="inlineStr">
         <is>
-          <t>[0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23]</t>
+          <t>[24,25,26,27]</t>
         </is>
       </c>
       <c r="H33" s="33" t="inlineStr">
@@ -11494,7 +11494,7 @@
       </c>
       <c r="G48" s="63" t="inlineStr">
         <is>
-          <t>all</t>
+          <t>[0:19)</t>
         </is>
       </c>
       <c r="H48" s="33" t="inlineStr">
@@ -17727,7 +17727,7 @@
       </c>
       <c r="D183" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="I183" s="56" t="n"/>
@@ -17740,7 +17740,7 @@
       </c>
       <c r="D184" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="I184" s="56" t="n"/>
@@ -17753,7 +17753,7 @@
       </c>
       <c r="D185" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E185" s="52" t="n"/>
@@ -17821,7 +17821,7 @@
       </c>
       <c r="D189" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J189" s="50" t="n"/>
@@ -17834,7 +17834,7 @@
       </c>
       <c r="D190" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J190" s="50" t="n"/>
@@ -17847,7 +17847,7 @@
       </c>
       <c r="D191" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E191" s="52" t="n"/>
@@ -17861,7 +17861,7 @@
       </c>
       <c r="D192" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E192" s="52" t="n"/>
@@ -17899,7 +17899,7 @@
       </c>
       <c r="D194" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E194" s="52" t="n"/>
@@ -17918,7 +17918,7 @@
       </c>
       <c r="D195" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E195" s="52" t="n"/>

</xml_diff>

<commit_message>
changed ride sharing occupancy rate from multiplier to adding increment.
</commit_message>
<xml_diff>
--- a/RECC_Config_V2_4.xlsx
+++ b/RECC_Config_V2_4.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9405" windowWidth="20730" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="4" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9405" windowWidth="20730" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cover" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Config_Sandbox" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" calcOnSave="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -1485,8 +1485,8 @@
     <col bestFit="1" customWidth="1" max="9" min="9" style="53" width="8.265625"/>
     <col customWidth="1" max="10" min="10" style="55" width="39.86328125"/>
     <col customWidth="1" max="11" min="11" style="53" width="46.73046875"/>
-    <col customWidth="1" max="57" min="12" style="53" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="58" style="53" width="10.6640625"/>
+    <col customWidth="1" max="59" min="12" style="53" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="60" style="53" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="8">
@@ -1886,8 +1886,8 @@
   </sheetPr>
   <dimension ref="A2:Q222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B180" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
-      <selection activeCell="C215" sqref="C215"/>
+    <sheetView topLeftCell="C73" workbookViewId="0" zoomScale="85" zoomScaleNormal="85">
+      <selection activeCell="I77" sqref="I77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -1906,8 +1906,8 @@
     <col customWidth="1" max="12" min="12" style="68" width="15.53125"/>
     <col customWidth="1" max="13" min="13" style="68" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="68" width="90"/>
-    <col customWidth="1" max="96" min="15" style="68" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="97" style="68" width="10.6640625"/>
+    <col customWidth="1" max="98" min="15" style="68" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="99" style="68" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -4065,7 +4065,7 @@
       </c>
       <c r="I80" s="29" t="inlineStr">
         <is>
-          <t>3d7b8c27-f22c-42f8-be81-09589a4308eb</t>
+          <t>eb5b84f4-b288-46ef-a3cc-eeb9737dbfb0</t>
         </is>
       </c>
       <c r="J80" t="inlineStr">
@@ -4686,7 +4686,7 @@
       </c>
       <c r="I91" s="29" t="inlineStr">
         <is>
-          <t>e57ce987-d7fa-4a43-a710-eb42610c859d</t>
+          <t>f4c746dd-b6cc-483e-9d3c-1e3b6f361c84</t>
         </is>
       </c>
       <c r="J91" t="inlineStr">
@@ -5116,7 +5116,7 @@
       </c>
       <c r="I99" s="29" t="inlineStr">
         <is>
-          <t>65738ce3-9052-4f6a-8a3a-2fb6ea0eed1e</t>
+          <t>157e822f-80a7-4fe1-a774-eb382556a99e</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -7547,7 +7547,7 @@
       </c>
       <c r="I143" s="29" t="inlineStr">
         <is>
-          <t>bf2da225-58ee-4419-b8ba-d6005808d227</t>
+          <t>09f30b78-0552-4644-bf3a-c24a3737049a</t>
         </is>
       </c>
       <c r="J143" t="inlineStr">
@@ -7601,7 +7601,7 @@
       </c>
       <c r="I144" s="29" t="inlineStr">
         <is>
-          <t>b2ab2c2b-8471-46c1-ae33-251c2bb271bf</t>
+          <t>4071bfc7-73e4-4415-9a1c-fd8c7091373f</t>
         </is>
       </c>
       <c r="J144" t="inlineStr">
@@ -8315,7 +8315,7 @@
       </c>
       <c r="I157" s="29" t="inlineStr">
         <is>
-          <t>a7c699a7-0ac8-45f2-9a1c-78913b472a82</t>
+          <t>e8782126-cf9c-4958-b1d0-f142667a5f66</t>
         </is>
       </c>
       <c r="J157" t="inlineStr">
@@ -8323,10 +8323,8 @@
           <t>SSP/RCP</t>
         </is>
       </c>
-      <c r="K157" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
+      <c r="K157" s="52" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="158">
@@ -8734,7 +8732,7 @@
       </c>
       <c r="E165" s="63" t="inlineStr">
         <is>
-          <t>V1.0</t>
+          <t>V1.1</t>
         </is>
       </c>
       <c r="F165" s="36" t="inlineStr">
@@ -8754,7 +8752,7 @@
       </c>
       <c r="I165" t="inlineStr">
         <is>
-          <t>d5553445-c90f-4422-bf80-94640f68ab2c</t>
+          <t>3586fa40-404b-4f4b-afbb-ce76c5cf5402</t>
         </is>
       </c>
       <c r="J165" t="inlineStr">
@@ -10139,8 +10137,8 @@
   </sheetPr>
   <dimension ref="A2:Q222"/>
   <sheetViews>
-    <sheetView topLeftCell="C165" workbookViewId="0">
-      <selection activeCell="I146" sqref="I146"/>
+    <sheetView topLeftCell="C60" workbookViewId="0">
+      <selection activeCell="H79" sqref="H79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -10159,8 +10157,8 @@
     <col customWidth="1" max="12" min="12" style="68" width="15.53125"/>
     <col customWidth="1" max="13" min="13" style="68" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="68" width="90"/>
-    <col customWidth="1" max="96" min="15" style="68" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="97" style="68" width="10.6640625"/>
+    <col customWidth="1" max="98" min="15" style="68" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="99" style="68" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -10236,7 +10234,7 @@
       </c>
       <c r="D7" s="63" t="inlineStr">
         <is>
-          <t>Germany_detail</t>
+          <t>Global</t>
         </is>
       </c>
     </row>
@@ -10548,7 +10546,7 @@
       </c>
       <c r="G21" s="63" t="inlineStr">
         <is>
-          <t>[33]</t>
+          <t>[2,13,31,32,33,34,35,36,37,38,39,9,4,12,40,41,42,43,44,45]</t>
         </is>
       </c>
       <c r="H21" s="33" t="inlineStr">
@@ -10771,7 +10769,7 @@
       </c>
       <c r="G27" s="63" t="inlineStr">
         <is>
-          <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58]</t>
+          <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34]</t>
         </is>
       </c>
       <c r="H27" s="33" t="inlineStr">
@@ -10808,7 +10806,7 @@
       </c>
       <c r="G28" s="63" t="inlineStr">
         <is>
-          <t>[0,2,3]</t>
+          <t>[0,2]</t>
         </is>
       </c>
       <c r="H28" s="33" t="inlineStr">
@@ -10845,7 +10843,7 @@
       </c>
       <c r="G29" s="63" t="inlineStr">
         <is>
-          <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58]</t>
+          <t>[0,1,2,3,4,5,22,23,24,25,26,27,28,29,30,31,32,33,34]</t>
         </is>
       </c>
       <c r="H29" s="33" t="inlineStr">
@@ -10993,7 +10991,7 @@
       </c>
       <c r="G33" s="63" t="inlineStr">
         <is>
-          <t>[0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23]</t>
+          <t>[24,25,26,27]</t>
         </is>
       </c>
       <c r="H33" s="33" t="inlineStr">
@@ -11548,7 +11546,7 @@
       </c>
       <c r="G48" s="63" t="inlineStr">
         <is>
-          <t>all</t>
+          <t>[0:19)</t>
         </is>
       </c>
       <c r="H48" s="33" t="inlineStr">
@@ -12319,7 +12317,7 @@
       </c>
       <c r="I80" s="29" t="inlineStr">
         <is>
-          <t>3d7b8c27-f22c-42f8-be81-09589a4308eb</t>
+          <t>eb5b84f4-b288-46ef-a3cc-eeb9737dbfb0</t>
         </is>
       </c>
       <c r="J80" t="inlineStr">
@@ -12940,7 +12938,7 @@
       </c>
       <c r="I91" s="29" t="inlineStr">
         <is>
-          <t>e57ce987-d7fa-4a43-a710-eb42610c859d</t>
+          <t>f4c746dd-b6cc-483e-9d3c-1e3b6f361c84</t>
         </is>
       </c>
       <c r="J91" t="inlineStr">
@@ -13370,7 +13368,7 @@
       </c>
       <c r="I99" s="29" t="inlineStr">
         <is>
-          <t>65738ce3-9052-4f6a-8a3a-2fb6ea0eed1e</t>
+          <t>157e822f-80a7-4fe1-a774-eb382556a99e</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -15801,7 +15799,7 @@
       </c>
       <c r="I143" s="29" t="inlineStr">
         <is>
-          <t>bf2da225-58ee-4419-b8ba-d6005808d227</t>
+          <t>09f30b78-0552-4644-bf3a-c24a3737049a</t>
         </is>
       </c>
       <c r="J143" t="inlineStr">
@@ -15855,7 +15853,7 @@
       </c>
       <c r="I144" s="29" t="inlineStr">
         <is>
-          <t>b2ab2c2b-8471-46c1-ae33-251c2bb271bf</t>
+          <t>4071bfc7-73e4-4415-9a1c-fd8c7091373f</t>
         </is>
       </c>
       <c r="J144" t="inlineStr">
@@ -16569,7 +16567,7 @@
       </c>
       <c r="I157" s="29" t="inlineStr">
         <is>
-          <t>a7c699a7-0ac8-45f2-9a1c-78913b472a82</t>
+          <t>e8782126-cf9c-4958-b1d0-f142667a5f66</t>
         </is>
       </c>
       <c r="J157" t="inlineStr">
@@ -16577,10 +16575,8 @@
           <t>SSP/RCP</t>
         </is>
       </c>
-      <c r="K157" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
+      <c r="K157" s="52" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="158">
@@ -16988,7 +16984,7 @@
       </c>
       <c r="E165" s="63" t="inlineStr">
         <is>
-          <t>V1.0</t>
+          <t>V1.1</t>
         </is>
       </c>
       <c r="F165" s="36" t="inlineStr">
@@ -17008,7 +17004,7 @@
       </c>
       <c r="I165" t="inlineStr">
         <is>
-          <t>d5553445-c90f-4422-bf80-94640f68ab2c</t>
+          <t>3586fa40-404b-4f4b-afbb-ce76c5cf5402</t>
         </is>
       </c>
       <c r="J165" t="inlineStr">
@@ -17942,7 +17938,7 @@
       </c>
       <c r="D191" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="J191" s="50" t="n"/>
@@ -17969,7 +17965,7 @@
       </c>
       <c r="D193" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E193" s="52" t="n"/>
@@ -17988,7 +17984,7 @@
       </c>
       <c r="D194" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E194" s="52" t="n"/>
@@ -18007,7 +18003,7 @@
       </c>
       <c r="D195" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E195" s="52" t="n"/>
@@ -18026,7 +18022,7 @@
       </c>
       <c r="D196" s="63" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>True</t>
         </is>
       </c>
       <c r="E196" s="52" t="n"/>
@@ -18063,7 +18059,7 @@
       </c>
       <c r="D198" s="42" t="inlineStr">
         <is>
-          <t>['pav']</t>
+          <t>['pav','reb']</t>
         </is>
       </c>
       <c r="E198" s="52" t="n"/>
@@ -18313,7 +18309,7 @@
         </is>
       </c>
       <c r="D215" s="43" t="n">
-        <v>500</v>
+        <v>50</v>
       </c>
     </row>
     <row r="216">
@@ -18392,8 +18388,8 @@
   </sheetPr>
   <dimension ref="A2:Q222"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
-      <selection activeCell="I146" sqref="I146"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
+      <selection activeCell="I76" sqref="I76:K179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -18412,8 +18408,8 @@
     <col customWidth="1" max="12" min="12" style="68" width="15.53125"/>
     <col customWidth="1" max="13" min="13" style="68" width="39.86328125"/>
     <col customWidth="1" max="14" min="14" style="68" width="90"/>
-    <col customWidth="1" max="96" min="15" style="68" width="10.6640625"/>
-    <col customWidth="1" max="16384" min="97" style="68" width="10.6640625"/>
+    <col customWidth="1" max="98" min="15" style="68" width="10.6640625"/>
+    <col customWidth="1" max="16384" min="99" style="68" width="10.6640625"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -20572,7 +20568,7 @@
       </c>
       <c r="I80" s="29" t="inlineStr">
         <is>
-          <t>3d7b8c27-f22c-42f8-be81-09589a4308eb</t>
+          <t>eb5b84f4-b288-46ef-a3cc-eeb9737dbfb0</t>
         </is>
       </c>
       <c r="J80" t="inlineStr">
@@ -21193,7 +21189,7 @@
       </c>
       <c r="I91" s="29" t="inlineStr">
         <is>
-          <t>e57ce987-d7fa-4a43-a710-eb42610c859d</t>
+          <t>f4c746dd-b6cc-483e-9d3c-1e3b6f361c84</t>
         </is>
       </c>
       <c r="J91" t="inlineStr">
@@ -21623,7 +21619,7 @@
       </c>
       <c r="I99" s="29" t="inlineStr">
         <is>
-          <t>65738ce3-9052-4f6a-8a3a-2fb6ea0eed1e</t>
+          <t>157e822f-80a7-4fe1-a774-eb382556a99e</t>
         </is>
       </c>
       <c r="J99" t="inlineStr">
@@ -24054,7 +24050,7 @@
       </c>
       <c r="I143" s="29" t="inlineStr">
         <is>
-          <t>bf2da225-58ee-4419-b8ba-d6005808d227</t>
+          <t>09f30b78-0552-4644-bf3a-c24a3737049a</t>
         </is>
       </c>
       <c r="J143" t="inlineStr">
@@ -24108,7 +24104,7 @@
       </c>
       <c r="I144" s="29" t="inlineStr">
         <is>
-          <t>b2ab2c2b-8471-46c1-ae33-251c2bb271bf</t>
+          <t>4071bfc7-73e4-4415-9a1c-fd8c7091373f</t>
         </is>
       </c>
       <c r="J144" t="inlineStr">
@@ -24822,7 +24818,7 @@
       </c>
       <c r="I157" s="29" t="inlineStr">
         <is>
-          <t>a7c699a7-0ac8-45f2-9a1c-78913b472a82</t>
+          <t>e8782126-cf9c-4958-b1d0-f142667a5f66</t>
         </is>
       </c>
       <c r="J157" t="inlineStr">
@@ -24830,10 +24826,8 @@
           <t>SSP/RCP</t>
         </is>
       </c>
-      <c r="K157" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
+      <c r="K157" s="52" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="158">
@@ -25241,7 +25235,7 @@
       </c>
       <c r="E165" s="63" t="inlineStr">
         <is>
-          <t>V1.0</t>
+          <t>V1.1</t>
         </is>
       </c>
       <c r="F165" s="36" t="inlineStr">
@@ -25261,7 +25255,7 @@
       </c>
       <c r="I165" t="inlineStr">
         <is>
-          <t>d5553445-c90f-4422-bf80-94640f68ab2c</t>
+          <t>3586fa40-404b-4f4b-afbb-ce76c5cf5402</t>
         </is>
       </c>
       <c r="J165" t="inlineStr">

</xml_diff>

<commit_message>
Added eff-suff plot also for single sectors and changed implementation of no-EE scenario variant.
</commit_message>
<xml_diff>
--- a/RECC_Config_V2_4.xlsx
+++ b/RECC_Config_V2_4.xlsx
@@ -10234,7 +10234,7 @@
       </c>
       <c r="D7" s="63" t="inlineStr">
         <is>
-          <t>Global</t>
+          <t>Global_North</t>
         </is>
       </c>
     </row>
@@ -10546,7 +10546,7 @@
       </c>
       <c r="G21" s="63" t="inlineStr">
         <is>
-          <t>[2,13,31,32,33,34,35,36,37,38,39,9,4,12,40,41,42,43,44,45]</t>
+          <t>[2,13,31,32,33,34,35,36,37,38,39,9,4,40,41]</t>
         </is>
       </c>
       <c r="H21" s="33" t="inlineStr">

</xml_diff>